<commit_message>
profile input speed improved
</commit_message>
<xml_diff>
--- a/projects/rokig/input/SimulatorScenarios.xlsx
+++ b/projects/rokig/input/SimulatorScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/rokig/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B13C78-9766-F244-B146-A4CA5026CBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2B6118-4745-1D4A-9A91-0EBB1291B204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -774,450 +774,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
@@ -1788,6 +1344,450 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1802,46 +1802,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{76E9500B-9B93-104C-98A9-49589EC2A5F4}" name="Table3" displayName="Table3" ref="A1:N2" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{76E9500B-9B93-104C-98A9-49589EC2A5F4}" name="Table3" displayName="Table3" ref="A1:N2" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="A1:N2" xr:uid="{76E9500B-9B93-104C-98A9-49589EC2A5F4}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{55B9D266-51A1-5648-9453-AE47B770ACA3}" name="id" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{76BFBC5C-AE5B-7546-84E4-D9B200D94307}" name="start_year" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{CFA7AB78-772F-2940-9461-0BA39A8B4295}" name="end_year" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{79EB89AA-F372-4D4A-BA4C-4C2F58B0E3A9}" name="id_region" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{A91B9FF3-49EA-F846-8C35-E56226A77A6F}" name="building_num_min" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{5CE5C7B2-174A-4447-B823-29509EEADD4D}" name="building_num_max" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{F698D0BE-46CA-B347-940E-4E5A1010DA13}" name="optimal_heating_behavior_prob" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{3D12CB80-1135-CE42-AD78-714ACC7800FB}" name="id_scenario_energy_price_wholesale" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{47BCF808-DD96-674F-B684-B42E7BAF7F8A}" name="id_scenario_energy_price_tax_rate" dataDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{1CCF13BE-FA67-EF41-A706-FC81390233B3}" name="id_scenario_energy_price_mark_up" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{18EC444E-E888-2F4D-B5EB-C5DE7A9B6059}" name="id_scenario_energy_price_co2_emission" dataDxfId="41"/>
-    <tableColumn id="12" xr3:uid="{0529EEC8-A084-2F4B-88CE-72A6305BC58E}" name="id_scenario_energy_emission_factor" dataDxfId="40"/>
-    <tableColumn id="13" xr3:uid="{B26F8B9B-D337-E340-B141-AE6C84ED2DD5}" name="name" dataDxfId="39"/>
-    <tableColumn id="14" xr3:uid="{B20C29FC-29F4-D24E-8153-A74BA16620C6}" name="comment" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{55B9D266-51A1-5648-9453-AE47B770ACA3}" name="id" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{76BFBC5C-AE5B-7546-84E4-D9B200D94307}" name="start_year" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{CFA7AB78-772F-2940-9461-0BA39A8B4295}" name="end_year" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{79EB89AA-F372-4D4A-BA4C-4C2F58B0E3A9}" name="id_region" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{A91B9FF3-49EA-F846-8C35-E56226A77A6F}" name="building_num_min" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{5CE5C7B2-174A-4447-B823-29509EEADD4D}" name="building_num_max" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{F698D0BE-46CA-B347-940E-4E5A1010DA13}" name="optimal_heating_behavior_prob" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{3D12CB80-1135-CE42-AD78-714ACC7800FB}" name="id_scenario_energy_price_wholesale" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{47BCF808-DD96-674F-B684-B42E7BAF7F8A}" name="id_scenario_energy_price_tax_rate" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{1CCF13BE-FA67-EF41-A706-FC81390233B3}" name="id_scenario_energy_price_mark_up" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{18EC444E-E888-2F4D-B5EB-C5DE7A9B6059}" name="id_scenario_energy_price_co2_emission" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{0529EEC8-A084-2F4B-88CE-72A6305BC58E}" name="id_scenario_energy_emission_factor" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{B26F8B9B-D337-E340-B141-AE6C84ED2DD5}" name="name" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{B20C29FC-29F4-D24E-8153-A74BA16620C6}" name="comment" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:N402" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:N402" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A1:N402" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="building_num_min" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="building_num_max" dataDxfId="27"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="optimal_heating_behavior_prob" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="id_scenario_energy_price_wholesale" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_mark_up" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_emission_factor" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="name" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="comment" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="48"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="building_num_min" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="building_num_max" dataDxfId="46"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="optimal_heating_behavior_prob" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="id_scenario_energy_price_wholesale" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_mark_up" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_emission_factor" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="name" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="comment" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2131,7 +2131,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2247,7 +2247,7 @@
   <dimension ref="A1:N402"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:N5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
units added to the exported tables
</commit_message>
<xml_diff>
--- a/projects/rokig/input/SimulatorScenarios.xlsx
+++ b/projects/rokig/input/SimulatorScenarios.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/rokig/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E7B0A8-243F-1143-9AF3-DC53555ACC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CCB600-4E81-B942-B4A9-3E261537431D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="nuts3" sheetId="3" r:id="rId1"/>
-    <sheet name="test" sheetId="5" r:id="rId2"/>
+    <sheet name="test" sheetId="5" r:id="rId1"/>
+    <sheet name="nuts3" sheetId="3" r:id="rId2"/>
     <sheet name="test-Hessen" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -774,450 +774,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="8" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
@@ -1788,6 +1344,450 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1802,46 +1802,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:N402" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="A1:N402" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{76E9500B-9B93-104C-98A9-49589EC2A5F4}" name="Table3" displayName="Table3" ref="A1:N2" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="A1:N2" xr:uid="{76E9500B-9B93-104C-98A9-49589EC2A5F4}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="building_num_min" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="building_num_max" dataDxfId="27"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="optimal_heating_behavior_prob" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="id_scenario_energy_price_wholesale" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_mark_up" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_emission_factor" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="name" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="comment" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{55B9D266-51A1-5648-9453-AE47B770ACA3}" name="id" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{76BFBC5C-AE5B-7546-84E4-D9B200D94307}" name="start_year" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{CFA7AB78-772F-2940-9461-0BA39A8B4295}" name="end_year" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{79EB89AA-F372-4D4A-BA4C-4C2F58B0E3A9}" name="id_region" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{A91B9FF3-49EA-F846-8C35-E56226A77A6F}" name="building_num_min" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{5CE5C7B2-174A-4447-B823-29509EEADD4D}" name="building_num_max" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{F698D0BE-46CA-B347-940E-4E5A1010DA13}" name="optimal_heating_behavior_prob" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{3D12CB80-1135-CE42-AD78-714ACC7800FB}" name="id_scenario_energy_price_wholesale" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{47BCF808-DD96-674F-B684-B42E7BAF7F8A}" name="id_scenario_energy_price_tax_rate" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{1CCF13BE-FA67-EF41-A706-FC81390233B3}" name="id_scenario_energy_price_mark_up" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{18EC444E-E888-2F4D-B5EB-C5DE7A9B6059}" name="id_scenario_energy_price_co2_emission" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{0529EEC8-A084-2F4B-88CE-72A6305BC58E}" name="id_scenario_energy_emission_factor" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{B26F8B9B-D337-E340-B141-AE6C84ED2DD5}" name="name" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{B20C29FC-29F4-D24E-8153-A74BA16620C6}" name="comment" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{76E9500B-9B93-104C-98A9-49589EC2A5F4}" name="Table3" displayName="Table3" ref="A1:N2" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
-  <autoFilter ref="A1:N2" xr:uid="{76E9500B-9B93-104C-98A9-49589EC2A5F4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:N402" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+  <autoFilter ref="A1:N402" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{55B9D266-51A1-5648-9453-AE47B770ACA3}" name="id" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{76BFBC5C-AE5B-7546-84E4-D9B200D94307}" name="start_year" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{CFA7AB78-772F-2940-9461-0BA39A8B4295}" name="end_year" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{79EB89AA-F372-4D4A-BA4C-4C2F58B0E3A9}" name="id_region" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{A91B9FF3-49EA-F846-8C35-E56226A77A6F}" name="building_num_min" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{5CE5C7B2-174A-4447-B823-29509EEADD4D}" name="building_num_max" dataDxfId="46"/>
-    <tableColumn id="7" xr3:uid="{F698D0BE-46CA-B347-940E-4E5A1010DA13}" name="optimal_heating_behavior_prob" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{3D12CB80-1135-CE42-AD78-714ACC7800FB}" name="id_scenario_energy_price_wholesale" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{47BCF808-DD96-674F-B684-B42E7BAF7F8A}" name="id_scenario_energy_price_tax_rate" dataDxfId="43"/>
-    <tableColumn id="10" xr3:uid="{1CCF13BE-FA67-EF41-A706-FC81390233B3}" name="id_scenario_energy_price_mark_up" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{18EC444E-E888-2F4D-B5EB-C5DE7A9B6059}" name="id_scenario_energy_price_co2_emission" dataDxfId="41"/>
-    <tableColumn id="12" xr3:uid="{0529EEC8-A084-2F4B-88CE-72A6305BC58E}" name="id_scenario_energy_emission_factor" dataDxfId="40"/>
-    <tableColumn id="13" xr3:uid="{B26F8B9B-D337-E340-B141-AE6C84ED2DD5}" name="name" dataDxfId="39"/>
-    <tableColumn id="14" xr3:uid="{B20C29FC-29F4-D24E-8153-A74BA16620C6}" name="comment" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="48"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="building_num_min" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="building_num_max" dataDxfId="46"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="optimal_heating_behavior_prob" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="id_scenario_energy_price_wholesale" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_mark_up" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_emission_factor" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="name" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="comment" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2127,10 +2127,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="9" max="9" width="30.5" customWidth="1"/>
+    <col min="10" max="10" width="30.83203125" customWidth="1"/>
+    <col min="11" max="11" width="34.6640625" customWidth="1"/>
+    <col min="12" max="12" width="31.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>2019</v>
+      </c>
+      <c r="C2" s="15">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="15">
+        <v>9010101</v>
+      </c>
+      <c r="E2" s="15">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15">
+        <v>2</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="H2" s="15">
+        <v>1</v>
+      </c>
+      <c r="I2" s="15">
+        <v>1</v>
+      </c>
+      <c r="J2" s="15">
+        <v>1</v>
+      </c>
+      <c r="K2" s="15">
+        <v>1</v>
+      </c>
+      <c r="L2" s="15">
+        <v>2</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N402"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -19837,122 +19953,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="30.5" customWidth="1"/>
-    <col min="10" max="10" width="30.83203125" customWidth="1"/>
-    <col min="11" max="11" width="34.6640625" customWidth="1"/>
-    <col min="12" max="12" width="31.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
-        <v>1</v>
-      </c>
-      <c r="B2" s="15">
-        <v>2019</v>
-      </c>
-      <c r="C2" s="15">
-        <v>2019</v>
-      </c>
-      <c r="D2" s="15">
-        <v>9010101</v>
-      </c>
-      <c r="E2" s="15">
-        <v>1</v>
-      </c>
-      <c r="F2" s="15">
-        <v>2</v>
-      </c>
-      <c r="G2" s="15">
-        <v>0.6</v>
-      </c>
-      <c r="H2" s="15">
-        <v>1</v>
-      </c>
-      <c r="I2" s="15">
-        <v>1</v>
-      </c>
-      <c r="J2" s="15">
-        <v>1</v>
-      </c>
-      <c r="K2" s="15">
-        <v>1</v>
-      </c>
-      <c r="L2" s="15">
-        <v>2</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>